<commit_message>
changement de nom de l'unité expérimentale en parcelle unitaire
</commit_message>
<xml_diff>
--- a/grapevine_experimental_thesaurus.xlsx
+++ b/grapevine_experimental_thesaurus.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xdelpuech\OneDrive - vignevin.com\AgricultureNumerique\ProjetsEnCours\VITISDATACROP\05_TRAVAIL_EN_COURS\WP1.1 Harmonisation\Expérimentation\vitisdatacrop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Expérimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BF0404C-9599-4AFD-9C59-AEFE2A76E172}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thesaurus" sheetId="2" r:id="rId1"/>
     <sheet name="Feuil1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="134">
   <si>
     <t>study (en)</t>
   </si>
@@ -133,16 +133,10 @@
     <t>Experimental unit</t>
   </si>
   <si>
-    <t xml:space="preserve">L'unité expérimentale est l'unité élémentaire qui reçoit un traitement. Elle est constituée d'une certaine étendue de terrain et d'un certain nombre de plants. </t>
-  </si>
-  <si>
     <t>the smallest unit to which a treatment is applied (Casler, 2015)</t>
   </si>
   <si>
     <t>skos:ExactMatch ADONIS:Parcelle unitaire</t>
-  </si>
-  <si>
-    <t>http://opendata.inrae.fr/thesaurusINRAE/c_21450</t>
   </si>
   <si>
     <t>Traitement ou objet de référence. En matière agronomique, cela peut être une ou quelques variétés largement utilisées dans la région considérée, un ensemble de parcelles qui ne sont soumises à aucun des traitements étudiées, ou soumises à un traitement classique considéré comme point de comparaison.</t>
@@ -239,9 +233,6 @@
     <t>niveaux,variantes</t>
   </si>
   <si>
-    <t>parcelle unitaire,unité expérimentale</t>
-  </si>
-  <si>
     <t>parcelle utile,placette expérimentale,placette d'échantillonnage</t>
   </si>
   <si>
@@ -272,9 +263,6 @@
     <t>traitement</t>
   </si>
   <si>
-    <t>unité expérimentale</t>
-  </si>
-  <si>
     <t>témoin</t>
   </si>
   <si>
@@ -435,6 +423,15 @@
   </si>
   <si>
     <t>Un dictionnaire de données permet d’expliciter les variables mesurées. Par exemple, pour un fichier tabulé, il peut être nécessaire de spécifier les entêtes des colonnes, les unités utilisées, les acronymes, etc.</t>
+  </si>
+  <si>
+    <t>parcelle unitaire</t>
+  </si>
+  <si>
+    <t>parcelle élémentaire,unité expérimentale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La parcelle unitaire (ou élémentaire) est la plus petite unité expérimentale qui reçoit un traitement. Dans les essais au champ, elle est constituée d'une certaine étendue de terrain et d'un certain nombre de plants. </t>
   </si>
 </sst>
 </file>
@@ -898,63 +895,63 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="3"/>
-    <col min="2" max="2" width="21.26953125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="65.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="3"/>
+    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="65.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="69" style="3" customWidth="1"/>
     <col min="7" max="7" width="30" style="3" customWidth="1"/>
-    <col min="8" max="8" width="39.54296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="35" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64.26953125" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="3"/>
+    <col min="10" max="10" width="64.28515625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="50" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -963,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>
@@ -971,19 +968,19 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -997,18 +994,18 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="50" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -1027,16 +1024,16 @@
         <v>11</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="9" t="s">
@@ -1051,12 +1048,12 @@
       <c r="I5" s="7"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>14</v>
@@ -1065,7 +1062,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>16</v>
@@ -1075,12 +1072,12 @@
       <c r="I6" s="7"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="112.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
@@ -1095,19 +1092,19 @@
       <c r="G7" s="6"/>
       <c r="H7" s="8"/>
       <c r="I7" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>20</v>
@@ -1121,16 +1118,16 @@
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="50" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="9" t="s">
@@ -1143,19 +1140,19 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="50" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>25</v>
@@ -1171,16 +1168,16 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J10" s="11"/>
     </row>
-    <row r="11" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="9" t="s">
@@ -1197,123 +1194,121 @@
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="50" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="4"/>
       <c r="E13" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="4"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:10" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="6"/>
       <c r="H15" s="5"/>
       <c r="I15" s="7"/>
       <c r="J15" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="4"/>
@@ -1321,19 +1316,19 @@
       <c r="I16" s="7"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="4"/>
@@ -1341,236 +1336,235 @@
       <c r="I17" s="7"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="7"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="112.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="13" t="s">
+      <c r="E24" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="13" t="s">
+    </row>
+    <row r="28" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I28" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="3" t="s">
+    <row r="29" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J29" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I28" s="3" t="s">
+    </row>
+    <row r="30" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="50" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="D30" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J29" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="3" t="s">
+      <c r="I30" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D30" s="3" t="s">
+    </row>
+    <row r="31" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="E31" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="3" t="s">
+      <c r="I31" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="B32" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I18" r:id="rId1" display="http://open-library.cirad.fr/files/2/521__946767658.pdf_x000a_EquipeprojetAdonis.2013" xr:uid="{7E5DCFAC-DFDD-4443-A4D6-3E9365D5B6EA}"/>
-    <hyperlink ref="J12" r:id="rId2" xr:uid="{84F8431D-0701-4BB8-87A8-64DE59F673DC}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{019A189E-BA24-47E3-8AAC-BE23ADC1A1F3}"/>
-    <hyperlink ref="J15" r:id="rId4" display="http://opendata.inrae.fr/thesaurusINRAE/c_16979" xr:uid="{78293DF7-1FA7-465C-8988-6BCD958AE1F0}"/>
-    <hyperlink ref="I22" r:id="rId5" xr:uid="{B6B2B57E-FDA2-464C-BA3B-4CE75142173D}"/>
-    <hyperlink ref="J29" r:id="rId6" xr:uid="{2D14577F-F6DB-4198-AF64-C90D96DCF16B}"/>
-    <hyperlink ref="I30" r:id="rId7" xr:uid="{D8E028A0-C1FD-4D2A-878E-2FF09F2CF6FD}"/>
-    <hyperlink ref="I31" r:id="rId8" xr:uid="{E377614F-49C2-400E-AED4-9237944A745F}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{019A189E-BA24-47E3-8AAC-BE23ADC1A1F3}"/>
+    <hyperlink ref="J15" r:id="rId3" display="http://opendata.inrae.fr/thesaurusINRAE/c_16979" xr:uid="{78293DF7-1FA7-465C-8988-6BCD958AE1F0}"/>
+    <hyperlink ref="I22" r:id="rId4" xr:uid="{B6B2B57E-FDA2-464C-BA3B-4CE75142173D}"/>
+    <hyperlink ref="J29" r:id="rId5" xr:uid="{2D14577F-F6DB-4198-AF64-C90D96DCF16B}"/>
+    <hyperlink ref="I30" r:id="rId6" xr:uid="{D8E028A0-C1FD-4D2A-878E-2FF09F2CF6FD}"/>
+    <hyperlink ref="I31" r:id="rId7" xr:uid="{E377614F-49C2-400E-AED4-9237944A745F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1580,7 +1574,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
integration des remarques sur doc en ligne, jusqu'à la table 3.2  incluse
</commit_message>
<xml_diff>
--- a/grapevine_experimental_thesaurus.xlsx
+++ b/grapevine_experimental_thesaurus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Expérimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BF0404C-9599-4AFD-9C59-AEFE2A76E172}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6C3B358-7D5B-4FDE-9EBF-F2D205EF2692}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2805" yWindow="4095" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thesaurus" sheetId="2" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Level</t>
   </si>
   <si>
-    <t>Chaque facteur étudié peut prendre plusieurs valeurs. Ces différentes valeurs liées à un facteur sont appelées, niveaux ou modalités. Le premier terme étant plutôt employé pour un facteur quantitatif et le deuxième pour un facteur qualitatif.</t>
-  </si>
-  <si>
     <t>a specific form or “state” of a factor (Casler, 2015)</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
   </si>
   <si>
     <t>Treatment</t>
-  </si>
-  <si>
-    <t>Toute modalité d'un facteur unique ou combinaison de modalités de deux ou plusieurs facteurs étudiés.</t>
   </si>
   <si>
     <t>a procedure or system whose effect on the experimental material is to be measured or observed (Casler, 2015)</t>
@@ -374,9 +368,6 @@
     <t>témoin non traité (TNT)</t>
   </si>
   <si>
-    <t>Traitement qui ne reçoit pas aucun des traitements phytosanitaires étudiés dans le cadre d'un essai d'évaluation biologique. L'objectif principal du témoin non traité est de qualifier le niveau d'infestation.</t>
-  </si>
-  <si>
     <t>EPPO.2006</t>
   </si>
   <si>
@@ -432,6 +423,15 @@
   </si>
   <si>
     <t xml:space="preserve">La parcelle unitaire (ou élémentaire) est la plus petite unité expérimentale qui reçoit un traitement. Dans les essais au champ, elle est constituée d'une certaine étendue de terrain et d'un certain nombre de plants. </t>
+  </si>
+  <si>
+    <t>Traitement qui ne reçoit pas aucun des traitements phytosanitaires étudiés dans le cadre d'un essai d'évaluation biologique. Un témoin non traité ne reçoit normalement aucun traitement contre l'organisme à étudier, avec pour objectif principal de qualifier le niveau d'infestation.</t>
+  </si>
+  <si>
+    <t>Chaque facteur étudié peut prendre plusieurs valeurs. Ces différentes valeurs liées à un facteur sont appelées niveaux ou modalités. Le premier terme étant plutôt employé pour un facteur quantitatif et le deuxième pour un facteur qualitatif.</t>
+  </si>
+  <si>
+    <t>Toute modalité (ou niveau) d'un facteur unique ou combinaison de modalités (ou niveaux) de deux ou plusieurs facteurs étudiés.</t>
   </si>
 </sst>
 </file>
@@ -895,8 +895,8 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -916,42 +916,42 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -960,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>
@@ -968,19 +968,19 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -994,7 +994,7 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>6</v>
@@ -1002,10 +1002,10 @@
     </row>
     <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -1024,16 +1024,16 @@
         <v>11</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="9" t="s">
@@ -1050,10 +1050,10 @@
     </row>
     <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>14</v>
@@ -1062,7 +1062,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>16</v>
@@ -1074,10 +1074,10 @@
     </row>
     <row r="7" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
@@ -1092,19 +1092,19 @@
       <c r="G7" s="6"/>
       <c r="H7" s="8"/>
       <c r="I7" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>20</v>
@@ -1118,16 +1118,16 @@
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="9" t="s">
@@ -1140,175 +1140,175 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="4"/>
       <c r="E13" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="4"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="6"/>
       <c r="H15" s="5"/>
       <c r="I15" s="7"/>
       <c r="J15" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="4"/>
@@ -1318,17 +1318,17 @@
     </row>
     <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="4"/>
@@ -1338,64 +1338,64 @@
     </row>
     <row r="18" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -1404,153 +1404,153 @@
     </row>
     <row r="21" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>97</v>
-      </c>
       <c r="E23" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="I30" s="14" t="s">
         <v>120</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I31" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change "traitement" to "traitement expérimental"
</commit_message>
<xml_diff>
--- a/grapevine_experimental_thesaurus.xlsx
+++ b/grapevine_experimental_thesaurus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Expérimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6C3B358-7D5B-4FDE-9EBF-F2D205EF2692}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8EF7F1F-5961-4F95-AF20-70D5D4F6530E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2805" yWindow="4095" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thesaurus" sheetId="2" r:id="rId1"/>
@@ -254,9 +254,6 @@
     <t>facteur non controlé</t>
   </si>
   <si>
-    <t>traitement</t>
-  </si>
-  <si>
     <t>témoin</t>
   </si>
   <si>
@@ -432,6 +429,9 @@
   </si>
   <si>
     <t>Toute modalité (ou niveau) d'un facteur unique ou combinaison de modalités (ou niveaux) de deux ou plusieurs facteurs étudiés.</t>
+  </si>
+  <si>
+    <t>traitement expérimental</t>
   </si>
 </sst>
 </file>
@@ -624,6 +624,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -895,8 +899,8 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -916,7 +920,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
@@ -948,7 +952,7 @@
     </row>
     <row r="2" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>66</v>
@@ -960,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>
@@ -974,13 +978,13 @@
     </row>
     <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -1002,7 +1006,7 @@
     </row>
     <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>68</v>
@@ -1030,7 +1034,7 @@
     </row>
     <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>69</v>
@@ -1050,7 +1054,7 @@
     </row>
     <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>70</v>
@@ -1062,7 +1066,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>16</v>
@@ -1074,7 +1078,7 @@
     </row>
     <row r="7" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>71</v>
@@ -1098,7 +1102,7 @@
     </row>
     <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>72</v>
@@ -1124,7 +1128,7 @@
     </row>
     <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>73</v>
@@ -1146,10 +1150,10 @@
     </row>
     <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>64</v>
@@ -1158,7 +1162,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>26</v>
@@ -1174,17 +1178,17 @@
     </row>
     <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>29</v>
@@ -1200,19 +1204,19 @@
     </row>
     <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>128</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>129</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>32</v>
@@ -1228,10 +1232,10 @@
     </row>
     <row r="13" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="4"/>
@@ -1248,10 +1252,10 @@
     </row>
     <row r="14" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
@@ -1274,10 +1278,10 @@
     </row>
     <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>65</v>
@@ -1286,7 +1290,7 @@
         <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="6"/>
@@ -1298,17 +1302,17 @@
     </row>
     <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="4"/>
@@ -1318,17 +1322,17 @@
     </row>
     <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="4"/>
@@ -1338,10 +1342,10 @@
     </row>
     <row r="18" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="9" t="s">
@@ -1364,10 +1368,10 @@
     </row>
     <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="4"/>
@@ -1384,10 +1388,10 @@
     </row>
     <row r="20" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
@@ -1404,153 +1408,153 @@
     </row>
     <row r="21" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="E22" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I22" s="14" t="s">
         <v>108</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B27" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>106</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J29" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="I30" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="I31" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update code and template
</commit_message>
<xml_diff>
--- a/grapevine_experimental_thesaurus.xlsx
+++ b/grapevine_experimental_thesaurus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Expérimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2508F006-4E47-4929-9C66-A275D3ED8D08}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79C83BAE-50CE-4A6A-A337-27E1C98EC3DB}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Thesaurus" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Thesaurus!$A$1:$K$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Thesaurus!$A$1:$L$38</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="190">
   <si>
     <t>study (en)</t>
   </si>
@@ -358,9 +358,6 @@
     <t>TNT</t>
   </si>
   <si>
-    <t>témoin non traité (TNT)</t>
-  </si>
-  <si>
     <t>EPPO.2006</t>
   </si>
   <si>
@@ -385,9 +382,6 @@
     <t>https://doranum.fr/plan-gestion-donnees-dmp/plan-de-gestion-des-donnees-fiche-synthetique_10_13143_cgv4-0k53/</t>
   </si>
   <si>
-    <t>Une expérimentation est une activité planifiée réalisée par un ensemble donné de personnes sur un ensemble donné d'unités d'observation, telles que des plantes, des placettes, des cuves…, impliquant un protocole, des méthodes et un jeu de données résultant</t>
-  </si>
-  <si>
     <t>jeu de données</t>
   </si>
   <si>
@@ -521,6 +515,93 @@
   </si>
   <si>
     <t>A field is a plot of land with the same plant population to which the same technical management is applied.</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>témoin non traité</t>
+  </si>
+  <si>
+    <t>Permanent sown grass</t>
+  </si>
+  <si>
+    <t>Permanent spontaneous cover crop</t>
+  </si>
+  <si>
+    <t>mechanical weeding</t>
+  </si>
+  <si>
+    <t>Chemical weed control</t>
+  </si>
+  <si>
+    <t>Heat weeding</t>
+  </si>
+  <si>
+    <t>mulching</t>
+  </si>
+  <si>
+    <t>enherbement semé</t>
+  </si>
+  <si>
+    <t>enherbement spontané</t>
+  </si>
+  <si>
+    <t>enherbement permanent</t>
+  </si>
+  <si>
+    <t>désherbage mécanique</t>
+  </si>
+  <si>
+    <t>désherbage chimique</t>
+  </si>
+  <si>
+    <t>désherbage thermique</t>
+  </si>
+  <si>
+    <t>paillage</t>
+  </si>
+  <si>
+    <t>http://opendata.inrae.fr/thesaurusINRAE/c_3045</t>
+  </si>
+  <si>
+    <t>http://opendata.inrae.fr/thesaurusINRAE/c_3170</t>
+  </si>
+  <si>
+    <t>http://opendata.inrae.fr/thesaurusINRAE/c_1940</t>
+  </si>
+  <si>
+    <t>enherbement temporaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’enherbement ou couvert végétal est issu d’un semis, et l’espèce ou les espèces semées dominent sa composition. </t>
+  </si>
+  <si>
+    <t>L’enherbement ou couvert végétal est composé en majorité d’espèces s’étant développées spontanément, il est parfois qualifié d'enherbement "naturel".</t>
+  </si>
+  <si>
+    <t>L’enherbement ou couvert végétal est présent tout au long de la saison.</t>
+  </si>
+  <si>
+    <t>L'enherbement ou couvert végétal est bien développé pendant la période de repos végétatif, puis est détruit en début de saison végétative, généralement autour du débourrement et au plus tard début floraison.</t>
+  </si>
+  <si>
+    <t>wikipedia, https://fr.wikipedia.org/wiki/D%C3%A9sherbage_thermique</t>
+  </si>
+  <si>
+    <t>Le désherbage thermique consiste à détruire les plantes indésirables (adventices) par choc thermique.</t>
+  </si>
+  <si>
+    <t>Le désherbage mécanique consiste à détruire les plantes indésirables (adventices) par des outils mécanisés qui bouleversent plus ou moins profondément la couche de surface du sol et affectent l'enracinement des adventices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le désherbage chimique consiste à détruire les plantes indésirables (adventices) ou à les empêcher de germer à l'aide de produits herbicides pulvérisés en surface. </t>
+  </si>
+  <si>
+    <t>Le paillage (ou mulchage) consiste à disposer une couche de matériau à la surface du sol, afin de protèger le sol et de maîtriser la germination et le développement des adventices par effet de barrière physique.</t>
+  </si>
+  <si>
+    <t>Une expérimentation est une activité planifiée consistant à observer un ensemble d'objets suivant un protocole préétabli pour tester une hypothèse, répondre à une question ou découvrir de nouveaux faits.</t>
   </si>
 </sst>
 </file>
@@ -982,37 +1063,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A05413-5B7D-41B8-9570-FC6697263454}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.453125" style="3"/>
-    <col min="3" max="3" width="21.26953125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="65.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="69" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30" style="3" customWidth="1"/>
-    <col min="9" max="9" width="39.54296875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="35" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="64.26953125" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="14.453125" style="3"/>
+    <col min="1" max="2" width="14.42578125" style="3"/>
+    <col min="3" max="3" width="21.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="65.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="69" style="3" customWidth="1"/>
+    <col min="9" max="9" width="30" style="3" customWidth="1"/>
+    <col min="10" max="10" width="39.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="35" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="64.28515625" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>48</v>
@@ -1020,34 +1102,37 @@
       <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>89</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>65</v>
@@ -1055,23 +1140,24 @@
       <c r="D2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="G2" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" ht="25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>89</v>
       </c>
@@ -1083,24 +1169,25 @@
         <v>101</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="50" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>89</v>
       </c>
@@ -1111,25 +1198,26 @@
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" spans="1:11" ht="25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>89</v>
       </c>
@@ -1138,24 +1226,25 @@
         <v>68</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>69</v>
@@ -1163,48 +1252,50 @@
       <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="112.5" x14ac:dyDescent="0.35">
+      <c r="J6" s="6"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>89</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>153</v>
-      </c>
       <c r="G7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="7" t="s">
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" spans="1:11" ht="25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>89</v>
       </c>
@@ -1215,23 +1306,24 @@
       <c r="D8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6"/>
+      <c r="K8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" ht="50" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>89</v>
       </c>
@@ -1240,21 +1332,22 @@
         <v>72</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6"/>
+      <c r="K9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" ht="50" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>89</v>
       </c>
@@ -1265,83 +1358,86 @@
       <c r="D10" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="G10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6"/>
+      <c r="K10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" ht="25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>89</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>129</v>
-      </c>
       <c r="G11" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="6"/>
+      <c r="K11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="6"/>
+      <c r="K12" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>89</v>
       </c>
@@ -1350,19 +1446,20 @@
         <v>73</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7" t="s">
+      <c r="H13" s="9"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>82</v>
       </c>
@@ -1370,25 +1467,26 @@
         <v>74</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="6"/>
+      <c r="J14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="K14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="K14" s="11"/>
-    </row>
-    <row r="15" spans="1:11" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>82</v>
       </c>
@@ -1398,26 +1496,27 @@
       <c r="D15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="11" t="s">
+      <c r="H15" s="4"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>84</v>
@@ -1425,21 +1524,22 @@
       <c r="D16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>161</v>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" ht="25" hidden="1" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>82</v>
       </c>
@@ -1451,16 +1551,17 @@
         <v>87</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="9"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
@@ -1468,25 +1569,26 @@
         <v>77</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="6"/>
+      <c r="F18" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="H18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="I18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="6"/>
+      <c r="K18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" ht="25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>82</v>
       </c>
@@ -1494,19 +1596,20 @@
         <v>78</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="4"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="6"/>
+      <c r="K19" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:11" ht="87.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>89</v>
       </c>
@@ -1515,19 +1618,20 @@
         <v>79</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="6"/>
+      <c r="H20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="6"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" ht="112.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="J20" s="6"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>89</v>
       </c>
@@ -1535,18 +1639,18 @@
       <c r="C21" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="G21" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="H21" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>90</v>
       </c>
@@ -1554,14 +1658,14 @@
       <c r="C22" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="G22" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="K22" s="14" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>90</v>
       </c>
@@ -1569,11 +1673,11 @@
       <c r="C23" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="G23" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>90</v>
       </c>
@@ -1581,11 +1685,11 @@
       <c r="C24" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="G24" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>90</v>
       </c>
@@ -1593,11 +1697,11 @@
       <c r="C25" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="G25" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>90</v>
       </c>
@@ -1606,7 +1710,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>90</v>
       </c>
@@ -1614,207 +1718,295 @@
       <c r="C27" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="G27" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="50" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="51" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="K28" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="J28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="50" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="s">
+      <c r="F29" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="H29" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L29" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="G29" s="3" t="s">
+    </row>
+    <row r="30" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="K29" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="B33" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="B35" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C35" s="3" t="s">
+    </row>
+    <row r="36" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F35" s="3" t="s">
+      <c r="F36" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="B36" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F36" s="3" t="s">
+      <c r="F37" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="H37" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="B37" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B38" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="G38" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>147</v>
+    </row>
+    <row r="39" spans="2:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C41" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="51" x14ac:dyDescent="0.25">
+      <c r="C43" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C45" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C46" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K38" xr:uid="{91A05413-5B7D-41B8-9570-FC6697263454}">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L38" xr:uid="{91A05413-5B7D-41B8-9570-FC6697263454}"/>
   <hyperlinks>
-    <hyperlink ref="J18" r:id="rId1" display="http://open-library.cirad.fr/files/2/521__946767658.pdf_x000a_EquipeprojetAdonis.2013" xr:uid="{7E5DCFAC-DFDD-4443-A4D6-3E9365D5B6EA}"/>
-    <hyperlink ref="K3" r:id="rId2" xr:uid="{019A189E-BA24-47E3-8AAC-BE23ADC1A1F3}"/>
-    <hyperlink ref="K15" r:id="rId3" display="http://opendata.inrae.fr/thesaurusINRAE/c_16979" xr:uid="{78293DF7-1FA7-465C-8988-6BCD958AE1F0}"/>
-    <hyperlink ref="J22" r:id="rId4" xr:uid="{B6B2B57E-FDA2-464C-BA3B-4CE75142173D}"/>
-    <hyperlink ref="K29" r:id="rId5" xr:uid="{2D14577F-F6DB-4198-AF64-C90D96DCF16B}"/>
-    <hyperlink ref="J30" r:id="rId6" xr:uid="{D8E028A0-C1FD-4D2A-878E-2FF09F2CF6FD}"/>
-    <hyperlink ref="J31" r:id="rId7" xr:uid="{E377614F-49C2-400E-AED4-9237944A745F}"/>
+    <hyperlink ref="K18" r:id="rId1" display="http://open-library.cirad.fr/files/2/521__946767658.pdf_x000a_EquipeprojetAdonis.2013" xr:uid="{7E5DCFAC-DFDD-4443-A4D6-3E9365D5B6EA}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{019A189E-BA24-47E3-8AAC-BE23ADC1A1F3}"/>
+    <hyperlink ref="L15" r:id="rId3" display="http://opendata.inrae.fr/thesaurusINRAE/c_16979" xr:uid="{78293DF7-1FA7-465C-8988-6BCD958AE1F0}"/>
+    <hyperlink ref="K22" r:id="rId4" xr:uid="{B6B2B57E-FDA2-464C-BA3B-4CE75142173D}"/>
+    <hyperlink ref="L29" r:id="rId5" xr:uid="{2D14577F-F6DB-4198-AF64-C90D96DCF16B}"/>
+    <hyperlink ref="K30" r:id="rId6" xr:uid="{D8E028A0-C1FD-4D2A-878E-2FF09F2CF6FD}"/>
+    <hyperlink ref="K31" r:id="rId7" xr:uid="{E377614F-49C2-400E-AED4-9237944A745F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
update to activate links in help page
</commit_message>
<xml_diff>
--- a/grapevine_experimental_thesaurus.xlsx
+++ b/grapevine_experimental_thesaurus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Expérimentation/vitisdatacrop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Experimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8820A835-1106-41CF-B324-C42FCE4D6C4E}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="13_ncr:1_{3E11090F-1850-41E8-9237-3A3D5692793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE9DF7AE-1977-447F-B778-ABBA1EF50431}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thesaurus" sheetId="2" r:id="rId1"/>
@@ -18,17 +18,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Thesaurus!$A$1:$L$38</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="227">
   <si>
     <t>study (en)</t>
   </si>
@@ -602,13 +613,124 @@
   </si>
   <si>
     <t>Une expérimentation est une activité planifiée consistant à observer un ensemble d'objets suivant un protocole préétabli pour tester une hypothèse, répondre à une question ou découvrir de nouveaux faits.</t>
+  </si>
+  <si>
+    <t>Agriculture biologique</t>
+  </si>
+  <si>
+    <t>Biodynamie</t>
+  </si>
+  <si>
+    <t>organic farming</t>
+  </si>
+  <si>
+    <t>Mode de production basé sur des pratiques agricoles qui excluent l’utilisation de biocides de synthèse et des organismes génétiquement modifiés (OGM) ou des produits obtenus à partir d’OGM.</t>
+  </si>
+  <si>
+    <t>http://opendata.inrae.fr/thesaurusINRAE/c_2912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode de gestion des productions agricoles, visant à minimiser l’impact de l’agriculture sur l’environnement en optimisant les intrants (produits phytosanitaires, fertilisants, aliments pour animaux, etc.) tout en maintenant, voire en améliorant la rentabilité économique des fermes. L’agriculture raisonnée est une démarche volontaire des agriculteurs qui souhaitent raisonner de façon globale à l’échelle de leur exploitation. </t>
+  </si>
+  <si>
+    <t>Agriculture raisonnée</t>
+  </si>
+  <si>
+    <t>http://opendata.inrae.fr/thesaurusINRAE/c_1593</t>
+  </si>
+  <si>
+    <t>Agriculture conventionelle</t>
+  </si>
+  <si>
+    <t>Mode de gestion des productions agricoles limitant la prise de risque</t>
+  </si>
+  <si>
+    <t>http://opendata.inrae.fr/thesaurusINRAE/c_3081</t>
+  </si>
+  <si>
+    <t>http://opendata.inrae.fr/thesaurusINRAE/c_1897</t>
+  </si>
+  <si>
+    <t>Forme d’agriculture biologique, qui se distingue par la mise en place de pratiques spécifiques, dont l’objectif est de favoriser la vitalité des plantes en renforçant le lien entre la plante, le sol et son environnement.</t>
+  </si>
+  <si>
+    <t>Denis, P., et al. (2022) Agriculture biodynamique : Définition. Dictionnaire d’agroécologie [Consulté le 08/07/22] https://doi.org/10.17180/dq6r-xg59 </t>
+  </si>
+  <si>
+    <t>Taille en gobelet</t>
+  </si>
+  <si>
+    <t>Cordon de Royat</t>
+  </si>
+  <si>
+    <t>Cordon double</t>
+  </si>
+  <si>
+    <t>Guyot simple</t>
+  </si>
+  <si>
+    <t>Guyot double</t>
+  </si>
+  <si>
+    <t>Guyot Poussard</t>
+  </si>
+  <si>
+    <t>Guyot mixte</t>
+  </si>
+  <si>
+    <t>Chablis</t>
+  </si>
+  <si>
+    <t>Taille rase de précision (mécanique)</t>
+  </si>
+  <si>
+    <t>Taille minimale (non-taille)</t>
+  </si>
+  <si>
+    <t>La souche à tronc court possède plusieurs bras, disposés dans le plan de palissage, terminés par des baguettes à 4 ou 5 yeux.</t>
+  </si>
+  <si>
+    <t>Reynier A., Manuel de viticulture, 9ième édition. 2003.</t>
+  </si>
+  <si>
+    <t>La souche est constitué par un tronc à deux bras portant chacun un courson et un long bois.</t>
+  </si>
+  <si>
+    <t>La souche porte un courson à deux yeux et un long bois.</t>
+  </si>
+  <si>
+    <t>La souche porte plusieurs bras répartis dans l'espace portant un ou plusieurs coursons, plus rarement à long bois.</t>
+  </si>
+  <si>
+    <t>La souche est composé d'un tronc vertical, avec un bras horizontal qui porte des coursons.</t>
+  </si>
+  <si>
+    <t>La souche est composé d'un tronc vertical et se sépare en deux  bras horizontaux disposés de part et d'autre dans l'axe du palissage. Chaque bras porte des coursons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taille en Guyot simple à deux bras, dont l’un porte un courson, et le deuxième une baguette et un courson de rappel. On alterne la position de la baguette d’une année sur l’autre, afin de conserver un équilibre entre les deux parties de la souche. </t>
+  </si>
+  <si>
+    <t>https://www.vignevin-occitanie.com/fiches-pratiques/la-taille-longue-de-la-vigne-en-guyot/. Consulté le 2024-04-29</t>
+  </si>
+  <si>
+    <t>Taille en Guyot mixte, avec la particularité de positionner les plaies de taille sur la partie supérieure du cordon dans l'objectif de respecter les flux de sève.</t>
+  </si>
+  <si>
+    <t>La TRP ou Taille Rase de Précision est une taille mécanisée poussée à l’extrême. Cette taille rase de précision (TRP) se réalise à un ou deux yeux maximum, soit 2 cm environ au-dessus du cordon. Les sarments non coupés par la taille mécanique sont supprimés par une reprise rapide à la main.</t>
+  </si>
+  <si>
+    <t>https://www.vignevin-occitanie.com/fiches-pratiques/taille-en-haie-non-taille-trp/</t>
+  </si>
+  <si>
+    <t>La non-taille ou taille minimale (minimal pruning) consiste à ne plus tailler la vigne et à ne pratiquer que des rognages. L’architecture s’articule généralement autour d’un seul cordon situé à 1.5-1.8 m et d’un système de palissage robuste.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,6 +801,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF474B4F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -731,7 +859,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -775,6 +903,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" xr:uid="{4F7340D3-744B-4525-807D-0528C9BB964F}"/>
@@ -794,10 +923,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1066,30 +1191,30 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.453125" style="3"/>
-    <col min="3" max="3" width="21.26953125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="65.54296875" style="3" customWidth="1"/>
+    <col min="1" max="2" width="14.44140625" style="3"/>
+    <col min="3" max="3" width="21.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="65.5546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="69" style="3" customWidth="1"/>
     <col min="9" max="9" width="30" style="3" customWidth="1"/>
-    <col min="10" max="10" width="39.54296875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="39.5546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="35" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="64.26953125" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="14.453125" style="3"/>
+    <col min="12" max="12" width="64.21875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="14.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>81</v>
       </c>
@@ -1127,7 +1252,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="50" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>89</v>
       </c>
@@ -1157,7 +1282,7 @@
       </c>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>89</v>
       </c>
@@ -1187,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="50" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>89</v>
       </c>
@@ -1217,7 +1342,7 @@
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>89</v>
       </c>
@@ -1239,7 +1364,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>89</v>
       </c>
@@ -1267,7 +1392,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="112.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>89</v>
       </c>
@@ -1295,7 +1420,7 @@
       </c>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>89</v>
       </c>
@@ -1323,7 +1448,7 @@
       </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="50" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>89</v>
       </c>
@@ -1347,7 +1472,7 @@
       </c>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="1:12" ht="50" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>89</v>
       </c>
@@ -1377,7 +1502,7 @@
       </c>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>89</v>
       </c>
@@ -1405,7 +1530,7 @@
       </c>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>82</v>
       </c>
@@ -1437,7 +1562,7 @@
       </c>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:12" ht="50" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>89</v>
       </c>
@@ -1459,7 +1584,7 @@
       </c>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>82</v>
       </c>
@@ -1486,7 +1611,7 @@
       </c>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>82</v>
       </c>
@@ -1511,7 +1636,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>82</v>
       </c>
@@ -1539,7 +1664,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>82</v>
       </c>
@@ -1561,7 +1686,7 @@
       <c r="K17" s="7"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
@@ -1588,7 +1713,7 @@
       </c>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>82</v>
       </c>
@@ -1609,7 +1734,7 @@
       </c>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="1:12" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>89</v>
       </c>
@@ -1631,7 +1756,7 @@
       <c r="K20" s="7"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" ht="112.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>89</v>
       </c>
@@ -1650,7 +1775,7 @@
       </c>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>90</v>
       </c>
@@ -1665,7 +1790,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
         <v>90</v>
       </c>
@@ -1677,7 +1802,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>90</v>
       </c>
@@ -1689,7 +1814,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>90</v>
       </c>
@@ -1701,7 +1826,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>90</v>
       </c>
@@ -1710,7 +1835,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>90</v>
       </c>
@@ -1722,7 +1847,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="50" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>82</v>
       </c>
@@ -1739,7 +1864,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="50" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>148</v>
       </c>
@@ -1759,7 +1884,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
         <v>111</v>
       </c>
@@ -1776,7 +1901,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
         <v>116</v>
       </c>
@@ -1790,7 +1915,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="C32" s="3" t="s">
         <v>120</v>
       </c>
@@ -1798,7 +1923,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>148</v>
       </c>
@@ -1815,7 +1940,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>148</v>
       </c>
@@ -1835,7 +1960,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>148</v>
       </c>
@@ -1852,7 +1977,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>148</v>
       </c>
@@ -1869,7 +1994,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>148</v>
       </c>
@@ -1886,7 +2011,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>148</v>
       </c>
@@ -1903,7 +2028,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
         <v>169</v>
       </c>
@@ -1914,7 +2039,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="C40" s="3" t="s">
         <v>170</v>
       </c>
@@ -1925,7 +2050,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
         <v>171</v>
       </c>
@@ -1933,7 +2058,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
         <v>179</v>
       </c>
@@ -1941,7 +2066,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="2:12" ht="50" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:12" ht="52.8" x14ac:dyDescent="0.3">
       <c r="C43" s="3" t="s">
         <v>172</v>
       </c>
@@ -1955,7 +2080,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
         <v>173</v>
       </c>
@@ -1969,7 +2094,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
         <v>174</v>
       </c>
@@ -1983,7 +2108,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
         <v>175</v>
       </c>
@@ -1995,6 +2120,163 @@
       </c>
       <c r="L46" s="3" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="C47" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L47" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="C48" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="L48" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C49" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L49" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C50" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L50" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="C51" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="K51" s="13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="C52" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="C53" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="C54" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="K54" s="13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="C55" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="K55" s="13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C56" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="K56" s="14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="3:12" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="C57" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="58" spans="3:12" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="C58" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="K58" s="13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="59" spans="3:12" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="C59" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="K59" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="C60" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="K60" s="14" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2007,8 +2289,11 @@
     <hyperlink ref="L29" r:id="rId5" xr:uid="{2D14577F-F6DB-4198-AF64-C90D96DCF16B}"/>
     <hyperlink ref="K30" r:id="rId6" xr:uid="{D8E028A0-C1FD-4D2A-878E-2FF09F2CF6FD}"/>
     <hyperlink ref="K31" r:id="rId7" xr:uid="{E377614F-49C2-400E-AED4-9237944A745F}"/>
+    <hyperlink ref="K56" r:id="rId8" xr:uid="{9A5ADF55-0302-406B-A43F-3D99440C5906}"/>
+    <hyperlink ref="K59" r:id="rId9" xr:uid="{DB7B0915-1D46-44BA-A511-C18906D5C685}"/>
+    <hyperlink ref="K60" r:id="rId10" xr:uid="{FF4439D4-3917-4219-A5B6-3D0279F99E2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>